<commit_message>
Actualizados resultados de filtrado colaborativo
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Experimentos 9010 random testset\Graph-Recommendations\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B18CA8-7BF9-444B-9581-CDC0A01093AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9324"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">results!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">results!$A$1:$F$685</definedName>
     <definedName name="cf_item_12" localSheetId="0">results!$D$578:$I$580</definedName>
     <definedName name="cf_item_25" localSheetId="0">results!$D$584:$I$586</definedName>
     <definedName name="cf_item_rprec" localSheetId="0">results!$D$590:$I$592</definedName>
@@ -64,8 +65,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="cf-item_121" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="cf-item_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\cf\cf-item_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -82,7 +83,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="cf-item_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="cf-item_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\cf\cf-item_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -99,7 +100,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="cf-item_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="cf-item_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\cf\cf-item_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -116,7 +117,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="cf-user_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="cf-user_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\cf\cf-user_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -133,7 +134,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="cf-user_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="cf-user_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\cf\cf-user_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -150,7 +151,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="cf-user_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="cf-user_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\cf\cf-user_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -167,7 +168,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="decisionTree_items_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="decisionTree_items_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\dec_tree\decisionTree_items_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -181,7 +182,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="decisionTree_items_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="decisionTree_items_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\dec_tree\decisionTree_items_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -195,7 +196,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="decisionTree_items_rprecision1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" name="decisionTree_items_rprecision1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\dec_tree\decisionTree_items_rprecision.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -209,7 +210,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="decisionTree_users_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF0A000000}" name="decisionTree_users_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\dec_tree\decisionTree_users_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -223,7 +224,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="decisionTree_users_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="11" xr16:uid="{00000000-0015-0000-FFFF-FFFF0B000000}" name="decisionTree_users_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\dec_tree\decisionTree_users_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -237,7 +238,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="decisionTree_users_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF0C000000}" name="decisionTree_users_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\dec_tree\decisionTree_users_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -251,7 +252,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" name="item_highest_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="13" xr16:uid="{00000000-0015-0000-FFFF-FFFF0D000000}" name="item_highest_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\items-gr\item_highest_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -265,7 +266,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" name="item_highest_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="14" xr16:uid="{00000000-0015-0000-FFFF-FFFF0E000000}" name="item_highest_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\items-gr\item_highest_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -279,7 +280,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" name="item_highest_srprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="15" xr16:uid="{00000000-0015-0000-FFFF-FFFF0F000000}" name="item_highest_srprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\items-gr\item_highest_srprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -293,7 +294,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" name="item_positional-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="16" xr16:uid="{00000000-0015-0000-FFFF-FFFF10000000}" name="item_positional-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\items-gr\item_positional-vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -307,7 +308,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" name="item_positional-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="17" xr16:uid="{00000000-0015-0000-FFFF-FFFF11000000}" name="item_positional-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\items-gr\item_positional-vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -321,7 +322,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="18" name="item_positional-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="18" xr16:uid="{00000000-0015-0000-FFFF-FFFF12000000}" name="item_positional-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\items-gr\item_positional-vot_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -335,7 +336,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="19" name="item_simple-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="19" xr16:uid="{00000000-0015-0000-FFFF-FFFF13000000}" name="item_simple-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\items-gr\item_simple-vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -349,7 +350,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="20" name="item_simple-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="20" xr16:uid="{00000000-0015-0000-FFFF-FFFF14000000}" name="item_simple-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\items-gr\item_simple-vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -363,7 +364,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="21" name="item_simple-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="21" xr16:uid="{00000000-0015-0000-FFFF-FFFF15000000}" name="item_simple-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\items-gr\item_simple-vot_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -377,7 +378,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="22" name="item_weighted-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="22" xr16:uid="{00000000-0015-0000-FFFF-FFFF16000000}" name="item_weighted-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\items-gr\item_weighted-vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -391,7 +392,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="23" name="item_weighted-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="23" xr16:uid="{00000000-0015-0000-FFFF-FFFF17000000}" name="item_weighted-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\items-gr\item_weighted-vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -405,7 +406,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="24" name="item_weighted-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="24" xr16:uid="{00000000-0015-0000-FFFF-FFFF18000000}" name="item_weighted-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\items-gr\item_weighted-vot_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -419,7 +420,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="25" name="naive-bayes_items_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="25" xr16:uid="{00000000-0015-0000-FFFF-FFFF19000000}" name="naive-bayes_items_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\naive_bayes\naive-bayes_items_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -433,7 +434,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="26" name="user_highest_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="26" xr16:uid="{00000000-0015-0000-FFFF-FFFF1A000000}" name="user_highest_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\users-gr\user_highest_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -447,7 +448,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="27" name="user_highest_sim_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="27" xr16:uid="{00000000-0015-0000-FFFF-FFFF1B000000}" name="user_highest_sim_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\users-gr\user_highest_sim_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -461,7 +462,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="28" name="user_highest_sim_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="28" xr16:uid="{00000000-0015-0000-FFFF-FFFF1C000000}" name="user_highest_sim_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\users-gr\user_highest_sim_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -475,7 +476,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="29" name="user_positional_vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="29" xr16:uid="{00000000-0015-0000-FFFF-FFFF1D000000}" name="user_positional_vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\users-gr\user_positional_vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -489,7 +490,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="30" name="user_positional_vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="30" xr16:uid="{00000000-0015-0000-FFFF-FFFF1E000000}" name="user_positional_vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\users-gr\user_positional_vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -503,7 +504,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="31" name="user_positional_vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="31" xr16:uid="{00000000-0015-0000-FFFF-FFFF1F000000}" name="user_positional_vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\users-gr\user_positional_vot_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -517,7 +518,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="32" name="user_simple_vot-121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="32" xr16:uid="{00000000-0015-0000-FFFF-FFFF20000000}" name="user_simple_vot-121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\users-gr\user_simple_vot-12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -531,7 +532,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="33" name="user_simple_vot-251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="33" xr16:uid="{00000000-0015-0000-FFFF-FFFF21000000}" name="user_simple_vot-251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\users-gr\user_simple_vot-25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -545,7 +546,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="34" name="user_simple_vot-rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="34" xr16:uid="{00000000-0015-0000-FFFF-FFFF22000000}" name="user_simple_vot-rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\users-gr\user_simple_vot-rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -559,7 +560,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="35" name="user_weighted_vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="35" xr16:uid="{00000000-0015-0000-FFFF-FFFF23000000}" name="user_weighted_vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\users-gr\user_weighted_vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -573,7 +574,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="36" name="user_weighted_vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="36" xr16:uid="{00000000-0015-0000-FFFF-FFFF24000000}" name="user_weighted_vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\users-gr\user_weighted_vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -587,7 +588,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="37" name="user_weighted_vot_501" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="37" xr16:uid="{00000000-0015-0000-FFFF-FFFF25000000}" name="user_weighted_vot_501" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\users-gr\user_weighted_vot_50.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -709,7 +710,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -761,151 +762,151 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="naive-bayes_items_12" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-user_25" connectionId="5" xr16:uid="{00000000-0016-0000-0000-000024000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-user_25" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_positional-vot_12" connectionId="16" xr16:uid="{00000000-0016-0000-0000-00001B000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-item_25" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_items_rprecision" connectionId="9" xr16:uid="{00000000-0016-0000-0000-00001A000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-user_12" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_users_rprec" connectionId="12" xr16:uid="{00000000-0016-0000-0000-000019000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-item_12" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_positional-vot_25" connectionId="17" xr16:uid="{00000000-0016-0000-0000-000018000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_weighted-vot_12" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_simple-vot_12" connectionId="19" xr16:uid="{00000000-0016-0000-0000-000017000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_highest_srprec" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_positional_vot_12" connectionId="29" xr16:uid="{00000000-0016-0000-0000-000016000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_simple_vot-12" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_weighted-vot_25" connectionId="23" xr16:uid="{00000000-0016-0000-0000-000015000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_positional-vot_rprec" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_simple_vot-25" connectionId="33" xr16:uid="{00000000-0016-0000-0000-000014000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_simple_vot-rprec" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_highest_12" connectionId="26" xr16:uid="{00000000-0016-0000-0000-000013000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_highest_sim_25" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_simple-vot_25" connectionId="20" xr16:uid="{00000000-0016-0000-0000-000012000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_users_rprec" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-user_rprec" connectionId="6" xr16:uid="{00000000-0016-0000-0000-000023000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_simple_vot-25" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_positional_vot_25" connectionId="30" xr16:uid="{00000000-0016-0000-0000-000011000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_weighted-vot_25" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_items_12" connectionId="7" xr16:uid="{00000000-0016-0000-0000-000010000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_simple-vot_25" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_simple-vot_rprec" connectionId="21" xr16:uid="{00000000-0016-0000-0000-00000F000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_weighted_vot_12" connectionId="35" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_highest_sim_25" connectionId="27" xr16:uid="{00000000-0016-0000-0000-00000E000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_simple-vot_rprec" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_weighted_vot_50" connectionId="37" xr16:uid="{00000000-0016-0000-0000-00000D000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_weighted-vot_rprec" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_simple_vot-rprec" connectionId="34" xr16:uid="{00000000-0016-0000-0000-00000C000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_highest_sim_rprec" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_weighted-vot_rprec" connectionId="24" xr16:uid="{00000000-0016-0000-0000-00000B000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_positional-vot_12" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_simple_vot-12" connectionId="32" xr16:uid="{00000000-0016-0000-0000-00000A000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_highest_12" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_weighted-vot_12" connectionId="22" xr16:uid="{00000000-0016-0000-0000-000009000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_positional_vot_rprec" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-item_12" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000008000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_items_rprecision" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_weighted_vot_25" connectionId="36" xr16:uid="{00000000-0016-0000-0000-000022000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_positional_vot_25" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_highest_12" connectionId="13" xr16:uid="{00000000-0016-0000-0000-000007000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_weighted_vot_50" connectionId="37" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="naive-bayes_items_12" connectionId="25" xr16:uid="{00000000-0016-0000-0000-000006000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_simple-vot_12" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_highest_srprec" connectionId="15" xr16:uid="{00000000-0016-0000-0000-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_positional-vot_25" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_weighted_vot_12" connectionId="35" xr16:uid="{00000000-0016-0000-0000-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_highest_12" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-item_rprec" connectionId="3" xr16:uid="{00000000-0016-0000-0000-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_weighted_vot_25" connectionId="36" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_positional_vot_rprec" connectionId="31" xr16:uid="{00000000-0016-0000-0000-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_positional_vot_12" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_positional-vot_rprec" connectionId="18" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_highest_25" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-item_25" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_users_25" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_highest_sim_rprec" connectionId="28" xr16:uid="{00000000-0016-0000-0000-000021000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_items_25" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-user_12" connectionId="4" xr16:uid="{00000000-0016-0000-0000-000020000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_users_12" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_highest_25" connectionId="14" xr16:uid="{00000000-0016-0000-0000-00001F000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_items_12" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_users_12" connectionId="10" xr16:uid="{00000000-0016-0000-0000-00001E000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-user_rprec" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_items_25" connectionId="8" xr16:uid="{00000000-0016-0000-0000-00001D000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-item_rprec" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_users_25" connectionId="11" xr16:uid="{00000000-0016-0000-0000-00001C000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1170,11 +1171,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I685"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L687" sqref="L687"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17936,13 +17937,13 @@
         <v>25</v>
       </c>
       <c r="G578">
-        <v>0.89297658862876195</v>
+        <v>0.89130434782608603</v>
       </c>
       <c r="H578">
-        <v>0.56856187290969895</v>
+        <v>0.58751393534002205</v>
       </c>
       <c r="I578">
-        <v>0.53600125746987803</v>
+        <v>0.536023698796667</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.3">
@@ -17965,13 +17966,13 @@
         <v>25</v>
       </c>
       <c r="G579">
-        <v>0.94314381270903003</v>
+        <v>0.941471571906354</v>
       </c>
       <c r="H579">
-        <v>0.53177257525083499</v>
+        <v>0.53612040133779204</v>
       </c>
       <c r="I579">
-        <v>0.53600125746987803</v>
+        <v>0.536023698796667</v>
       </c>
     </row>
     <row r="580" spans="1:9" x14ac:dyDescent="0.3">
@@ -17994,13 +17995,13 @@
         <v>25</v>
       </c>
       <c r="G580">
-        <v>0.97826086956521696</v>
+        <v>0.97491638795986602</v>
       </c>
       <c r="H580">
-        <v>0.46070234113712299</v>
+        <v>0.459197324414715</v>
       </c>
       <c r="I580">
-        <v>0.53600125746987803</v>
+        <v>0.536023698796667</v>
       </c>
     </row>
     <row r="581" spans="1:9" x14ac:dyDescent="0.3">
@@ -18023,13 +18024,13 @@
         <v>25</v>
       </c>
       <c r="G581">
-        <v>0.89799331103678903</v>
+        <v>0.896321070234113</v>
       </c>
       <c r="H581">
-        <v>0.56633221850613202</v>
+        <v>0.56577480490524001</v>
       </c>
       <c r="I581">
-        <v>0.11043601975876199</v>
+        <v>0.110017959558093</v>
       </c>
     </row>
     <row r="582" spans="1:9" x14ac:dyDescent="0.3">
@@ -18052,13 +18053,13 @@
         <v>25</v>
       </c>
       <c r="G582">
-        <v>0.95652173913043403</v>
+        <v>0.95484949832775901</v>
       </c>
       <c r="H582">
         <v>0.54615384615384599</v>
       </c>
       <c r="I582">
-        <v>0.11043601975876199</v>
+        <v>0.110017959558093</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.3">
@@ -18084,10 +18085,10 @@
         <v>0.993311036789297</v>
       </c>
       <c r="H583">
-        <v>0.467391304347825</v>
+        <v>0.467892976588628</v>
       </c>
       <c r="I583">
-        <v>0.11043601975876199</v>
+        <v>0.110017959558093</v>
       </c>
     </row>
     <row r="584" spans="1:9" x14ac:dyDescent="0.3">
@@ -18110,13 +18111,13 @@
         <v>25</v>
       </c>
       <c r="G584">
-        <v>0.97872340425531901</v>
+        <v>0.97606382978723405</v>
       </c>
       <c r="H584">
-        <v>0.76684397163120499</v>
+        <v>0.76241134751772999</v>
       </c>
       <c r="I584">
-        <v>0.6264826631007</v>
+        <v>0.62396135535997799</v>
       </c>
     </row>
     <row r="585" spans="1:9" x14ac:dyDescent="0.3">
@@ -18142,10 +18143,10 @@
         <v>0.99202127659574402</v>
       </c>
       <c r="H585">
-        <v>0.68457446808510702</v>
+        <v>0.68457446808510602</v>
       </c>
       <c r="I585">
-        <v>0.6264826631007</v>
+        <v>0.62396135535997799</v>
       </c>
     </row>
     <row r="586" spans="1:9" x14ac:dyDescent="0.3">
@@ -18171,10 +18172,10 @@
         <v>0.99734042553191404</v>
       </c>
       <c r="H586">
-        <v>0.59388297872340401</v>
+        <v>0.59255319148936103</v>
       </c>
       <c r="I586">
-        <v>0.6264826631007</v>
+        <v>0.62396135535997799</v>
       </c>
     </row>
     <row r="587" spans="1:9" x14ac:dyDescent="0.3">
@@ -18200,7 +18201,7 @@
         <v>0.94680851063829696</v>
       </c>
       <c r="H587">
-        <v>0.64450354609928995</v>
+        <v>0.64539007092198497</v>
       </c>
       <c r="I587">
         <v>0.127276878706399</v>
@@ -18229,7 +18230,7 @@
         <v>0.98670212765957399</v>
       </c>
       <c r="H588">
-        <v>0.64414893617021296</v>
+        <v>0.64468085106383</v>
       </c>
       <c r="I588">
         <v>0.127276878706399</v>
@@ -18284,13 +18285,13 @@
         <v>25</v>
       </c>
       <c r="G590">
-        <v>0.95348837209302295</v>
+        <v>0.97674418604651103</v>
       </c>
       <c r="H590">
-        <v>0.70801033591731199</v>
+        <v>0.73126614987080096</v>
       </c>
       <c r="I590">
-        <v>0.66537269793083698</v>
+        <v>0.65547946885156105</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.3">
@@ -18313,13 +18314,13 @@
         <v>25</v>
       </c>
       <c r="G591">
-        <v>1</v>
+        <v>0.99224806201550297</v>
       </c>
       <c r="H591">
-        <v>0.70387596899224703</v>
+        <v>0.69767441860464996</v>
       </c>
       <c r="I591">
-        <v>0.66537269793083698</v>
+        <v>0.65547946885156105</v>
       </c>
     </row>
     <row r="592" spans="1:9" x14ac:dyDescent="0.3">
@@ -18345,10 +18346,10 @@
         <v>1</v>
       </c>
       <c r="H592">
-        <v>0.665116279069768</v>
+        <v>0.65891472868217005</v>
       </c>
       <c r="I592">
-        <v>0.66537269793083698</v>
+        <v>0.65547946885156105</v>
       </c>
     </row>
     <row r="593" spans="1:9" x14ac:dyDescent="0.3">
@@ -21049,9 +21050,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:F685" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="H1" r:id="rId1" display="P@k "/>
+    <hyperlink ref="H1" r:id="rId1" display="P@k " xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct typos in simple voting results for user-based graphs
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Experimentos 9010 random testset\Graph-Recommendations\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B18CA8-7BF9-444B-9581-CDC0A01093AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -49,7 +48,7 @@
     <definedName name="user_positional_vot_25" localSheetId="0">results!$D$362:$I$385</definedName>
     <definedName name="user_positional_vot_rprec" localSheetId="0">results!$D$554:$I$577</definedName>
     <definedName name="user_simple_vot_12" localSheetId="0">results!$D$122:$I$145</definedName>
-    <definedName name="user_simple_vot_25" localSheetId="0">results!$D$314:$I$337</definedName>
+    <definedName name="user_simple_vot_25" localSheetId="0">results!$D$314:$N$337</definedName>
     <definedName name="user_simple_vot_rprec" localSheetId="0">results!$D$506:$I$529</definedName>
     <definedName name="user_weighted_vot_12" localSheetId="0">results!$D$146:$I$169</definedName>
     <definedName name="user_weighted_vot_25" localSheetId="0">results!$D$338:$I$361</definedName>
@@ -65,8 +64,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="cf-item_121" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="cf-item_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\cf\cf-item_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -83,7 +82,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="cf-item_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="2" name="cf-item_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\cf\cf-item_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -100,7 +99,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="cf-item_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="3" name="cf-item_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\cf\cf-item_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -117,7 +116,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="cf-user_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="4" name="cf-user_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\cf\cf-user_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -134,7 +133,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="cf-user_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="5" name="cf-user_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\cf\cf-user_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -151,7 +150,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="cf-user_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="6" name="cf-user_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\cf\cf-user_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="11">
         <textField/>
@@ -168,7 +167,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="decisionTree_items_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="7" name="decisionTree_items_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\dec_tree\decisionTree_items_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -182,7 +181,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="decisionTree_items_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="8" name="decisionTree_items_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\dec_tree\decisionTree_items_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -196,7 +195,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" name="decisionTree_items_rprecision1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="9" name="decisionTree_items_rprecision1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\dec_tree\decisionTree_items_rprecision.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -210,7 +209,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF0A000000}" name="decisionTree_users_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="10" name="decisionTree_users_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\dec_tree\decisionTree_users_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -224,7 +223,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" xr16:uid="{00000000-0015-0000-FFFF-FFFF0B000000}" name="decisionTree_users_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="11" name="decisionTree_users_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\dec_tree\decisionTree_users_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -238,7 +237,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF0C000000}" name="decisionTree_users_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="12" name="decisionTree_users_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\dec_tree\decisionTree_users_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -252,7 +251,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" xr16:uid="{00000000-0015-0000-FFFF-FFFF0D000000}" name="item_highest_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="13" name="item_highest_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\items-gr\item_highest_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -266,7 +265,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" xr16:uid="{00000000-0015-0000-FFFF-FFFF0E000000}" name="item_highest_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="14" name="item_highest_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\items-gr\item_highest_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -280,7 +279,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" xr16:uid="{00000000-0015-0000-FFFF-FFFF0F000000}" name="item_highest_srprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="15" name="item_highest_srprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\items-gr\item_highest_srprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -294,7 +293,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" xr16:uid="{00000000-0015-0000-FFFF-FFFF10000000}" name="item_positional-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="16" name="item_positional-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\items-gr\item_positional-vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -308,7 +307,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" xr16:uid="{00000000-0015-0000-FFFF-FFFF11000000}" name="item_positional-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="17" name="item_positional-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\items-gr\item_positional-vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -322,7 +321,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="18" xr16:uid="{00000000-0015-0000-FFFF-FFFF12000000}" name="item_positional-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="18" name="item_positional-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\items-gr\item_positional-vot_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -336,7 +335,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="19" xr16:uid="{00000000-0015-0000-FFFF-FFFF13000000}" name="item_simple-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="19" name="item_simple-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\items-gr\item_simple-vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -350,7 +349,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="20" xr16:uid="{00000000-0015-0000-FFFF-FFFF14000000}" name="item_simple-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="20" name="item_simple-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\items-gr\item_simple-vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -364,7 +363,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="21" xr16:uid="{00000000-0015-0000-FFFF-FFFF15000000}" name="item_simple-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="21" name="item_simple-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\items-gr\item_simple-vot_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -378,7 +377,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="22" xr16:uid="{00000000-0015-0000-FFFF-FFFF16000000}" name="item_weighted-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="22" name="item_weighted-vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\items-gr\item_weighted-vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -392,7 +391,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="23" xr16:uid="{00000000-0015-0000-FFFF-FFFF17000000}" name="item_weighted-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="23" name="item_weighted-vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\items-gr\item_weighted-vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -406,7 +405,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="24" xr16:uid="{00000000-0015-0000-FFFF-FFFF18000000}" name="item_weighted-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="24" name="item_weighted-vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\items-gr\item_weighted-vot_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -420,7 +419,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="25" xr16:uid="{00000000-0015-0000-FFFF-FFFF19000000}" name="naive-bayes_items_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="25" name="naive-bayes_items_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\naive_bayes\naive-bayes_items_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -434,7 +433,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="26" xr16:uid="{00000000-0015-0000-FFFF-FFFF1A000000}" name="user_highest_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="26" name="user_highest_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\users-gr\user_highest_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -448,7 +447,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="27" xr16:uid="{00000000-0015-0000-FFFF-FFFF1B000000}" name="user_highest_sim_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="27" name="user_highest_sim_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\users-gr\user_highest_sim_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -462,7 +461,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="28" xr16:uid="{00000000-0015-0000-FFFF-FFFF1C000000}" name="user_highest_sim_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="28" name="user_highest_sim_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\users-gr\user_highest_sim_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -476,7 +475,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="29" xr16:uid="{00000000-0015-0000-FFFF-FFFF1D000000}" name="user_positional_vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="29" name="user_positional_vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\users-gr\user_positional_vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -490,7 +489,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="30" xr16:uid="{00000000-0015-0000-FFFF-FFFF1E000000}" name="user_positional_vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="30" name="user_positional_vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\users-gr\user_positional_vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -504,7 +503,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="31" xr16:uid="{00000000-0015-0000-FFFF-FFFF1F000000}" name="user_positional_vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="31" name="user_positional_vot_rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\users-gr\user_positional_vot_rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -518,7 +517,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="32" xr16:uid="{00000000-0015-0000-FFFF-FFFF20000000}" name="user_simple_vot-121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="32" name="user_simple_vot-121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\users-gr\user_simple_vot-12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -532,7 +531,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="33" xr16:uid="{00000000-0015-0000-FFFF-FFFF21000000}" name="user_simple_vot-251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="33" name="user_simple_vot-251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\users-gr\user_simple_vot-25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -546,7 +545,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="34" xr16:uid="{00000000-0015-0000-FFFF-FFFF22000000}" name="user_simple_vot-rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="34" name="user_simple_vot-rprec1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\users-gr\user_simple_vot-rprec.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -560,7 +559,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="35" xr16:uid="{00000000-0015-0000-FFFF-FFFF23000000}" name="user_weighted_vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="35" name="user_weighted_vot_121" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\12%\users-gr\user_weighted_vot_12.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -574,7 +573,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="36" xr16:uid="{00000000-0015-0000-FFFF-FFFF24000000}" name="user_weighted_vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="36" name="user_weighted_vot_251" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\25%\users-gr\user_weighted_vot_25.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -588,7 +587,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="37" xr16:uid="{00000000-0015-0000-FFFF-FFFF25000000}" name="user_weighted_vot_501" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="37" name="user_weighted_vot_501" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\50%\users-gr\user_weighted_vot_50.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="8">
         <textField/>
@@ -710,7 +709,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -762,151 +761,151 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-user_25" connectionId="5" xr16:uid="{00000000-0016-0000-0000-000024000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_positional_vot_12" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_positional-vot_12" connectionId="16" xr16:uid="{00000000-0016-0000-0000-00001B000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_positional_vot_25" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_items_rprecision" connectionId="9" xr16:uid="{00000000-0016-0000-0000-00001A000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_simple_vot-rprec" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_users_rprec" connectionId="12" xr16:uid="{00000000-0016-0000-0000-000019000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_simple_vot-25" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_positional-vot_25" connectionId="17" xr16:uid="{00000000-0016-0000-0000-000018000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_users_rprec" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_simple-vot_12" connectionId="19" xr16:uid="{00000000-0016-0000-0000-000017000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-user_rprec" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_positional_vot_12" connectionId="29" xr16:uid="{00000000-0016-0000-0000-000016000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_users_12" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_weighted-vot_25" connectionId="23" xr16:uid="{00000000-0016-0000-0000-000015000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-item_rprec" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_simple_vot-25" connectionId="33" xr16:uid="{00000000-0016-0000-0000-000014000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-item_12" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_highest_12" connectionId="26" xr16:uid="{00000000-0016-0000-0000-000013000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_weighted-vot_rprec" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_simple-vot_25" connectionId="20" xr16:uid="{00000000-0016-0000-0000-000012000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_items_12" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-user_rprec" connectionId="6" xr16:uid="{00000000-0016-0000-0000-000023000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-user_25" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_positional_vot_25" connectionId="30" xr16:uid="{00000000-0016-0000-0000-000011000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_positional-vot_25" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_items_12" connectionId="7" xr16:uid="{00000000-0016-0000-0000-000010000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_items_25" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_simple-vot_rprec" connectionId="21" xr16:uid="{00000000-0016-0000-0000-00000F000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_weighted_vot_25" connectionId="36" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_highest_sim_25" connectionId="27" xr16:uid="{00000000-0016-0000-0000-00000E000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_highest_12" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_weighted_vot_50" connectionId="37" xr16:uid="{00000000-0016-0000-0000-00000D000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_highest_12" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_simple_vot-rprec" connectionId="34" xr16:uid="{00000000-0016-0000-0000-00000C000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_users_25" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_weighted-vot_rprec" connectionId="24" xr16:uid="{00000000-0016-0000-0000-00000B000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_positional_vot_rprec" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_simple_vot-12" connectionId="32" xr16:uid="{00000000-0016-0000-0000-00000A000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_simple_vot-12" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_weighted-vot_12" connectionId="22" xr16:uid="{00000000-0016-0000-0000-000009000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_simple-vot_rprec" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-item_12" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000008000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_simple-vot_12" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_weighted_vot_25" connectionId="36" xr16:uid="{00000000-0016-0000-0000-000022000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-item_25" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_highest_12" connectionId="13" xr16:uid="{00000000-0016-0000-0000-000007000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_highest_sim_rprec" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="naive-bayes_items_12" connectionId="25" xr16:uid="{00000000-0016-0000-0000-000006000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_positional-vot_rprec" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_highest_srprec" connectionId="15" xr16:uid="{00000000-0016-0000-0000-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="naive-bayes_items_12" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_weighted_vot_12" connectionId="35" xr16:uid="{00000000-0016-0000-0000-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_highest_sim_25" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-item_rprec" connectionId="3" xr16:uid="{00000000-0016-0000-0000-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_positional-vot_12" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_positional_vot_rprec" connectionId="31" xr16:uid="{00000000-0016-0000-0000-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cf-user_12" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_positional-vot_rprec" connectionId="18" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_weighted-vot_12" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-item_25" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_simple-vot_25" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="user_highest_sim_rprec" connectionId="28" xr16:uid="{00000000-0016-0000-0000-000021000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_highest_srprec" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cf-user_12" connectionId="4" xr16:uid="{00000000-0016-0000-0000-000020000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_weighted_vot_50" connectionId="37" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="item_highest_25" connectionId="14" xr16:uid="{00000000-0016-0000-0000-00001F000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_weighted-vot_25" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_users_12" connectionId="10" xr16:uid="{00000000-0016-0000-0000-00001E000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="decisionTree_items_rprecision" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_items_25" connectionId="8" xr16:uid="{00000000-0016-0000-0000-00001D000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="item_highest_25" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="decisionTree_users_25" connectionId="11" xr16:uid="{00000000-0016-0000-0000-00001C000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="user_weighted_vot_12" connectionId="35" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1171,11 +1170,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I685"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L687" sqref="L687"/>
+    <sheetView tabSelected="1" topLeftCell="A307" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M332" sqref="M332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10281,13 +10280,13 @@
         <v>15</v>
       </c>
       <c r="G314">
-        <v>0.73138297872340396</v>
+        <v>0.96808510638297796</v>
       </c>
       <c r="H314">
-        <v>0.24379432624113401</v>
+        <v>0.76418439716312003</v>
       </c>
       <c r="I314">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.3">
@@ -10310,13 +10309,13 @@
         <v>15</v>
       </c>
       <c r="G315">
-        <v>0.73138297872340396</v>
+        <v>0.96808510638297796</v>
       </c>
       <c r="H315">
-        <v>0.24379432624113401</v>
+        <v>0.76418439716312003</v>
       </c>
       <c r="I315">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.3">
@@ -10339,13 +10338,13 @@
         <v>15</v>
       </c>
       <c r="G316">
-        <v>0.73138297872340396</v>
+        <v>0.96808510638297796</v>
       </c>
       <c r="H316">
-        <v>0.24379432624113401</v>
+        <v>0.76418439716312003</v>
       </c>
       <c r="I316">
-        <v>0.22220744680851001</v>
+        <v>0.47451241134751798</v>
       </c>
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.3">
@@ -10368,13 +10367,13 @@
         <v>15</v>
       </c>
       <c r="G317">
-        <v>0.73138297872340396</v>
+        <v>0.96808510638297796</v>
       </c>
       <c r="H317">
-        <v>0.24379432624113401</v>
+        <v>0.76418439716312003</v>
       </c>
       <c r="I317">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.3">
@@ -10397,13 +10396,13 @@
         <v>15</v>
       </c>
       <c r="G318">
-        <v>0.73138297872340396</v>
+        <v>0.96808510638297796</v>
       </c>
       <c r="H318">
-        <v>0.24379432624113401</v>
+        <v>0.76418439716312003</v>
       </c>
       <c r="I318">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.3">
@@ -10426,13 +10425,13 @@
         <v>15</v>
       </c>
       <c r="G319">
-        <v>0.73138297872340396</v>
+        <v>0.96808510638297796</v>
       </c>
       <c r="H319">
-        <v>0.24379432624113401</v>
+        <v>0.76418439716312003</v>
       </c>
       <c r="I319">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.3">
@@ -10455,13 +10454,13 @@
         <v>15</v>
       </c>
       <c r="G320">
-        <v>0.73138297872340396</v>
+        <v>0.96808510638297796</v>
       </c>
       <c r="H320">
-        <v>0.24379432624113401</v>
+        <v>0.76418439716312003</v>
       </c>
       <c r="I320">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
@@ -10484,13 +10483,13 @@
         <v>15</v>
       </c>
       <c r="G321">
-        <v>0.73138297872340396</v>
+        <v>0.96808510638297796</v>
       </c>
       <c r="H321">
-        <v>0.24379432624113401</v>
+        <v>0.76418439716312003</v>
       </c>
       <c r="I321">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
@@ -10513,13 +10512,13 @@
         <v>15</v>
       </c>
       <c r="G322">
-        <v>0.73138297872340396</v>
+        <v>0.98138297872340396</v>
       </c>
       <c r="H322">
-        <v>0.14627659574468099</v>
+        <v>0.69095744680851101</v>
       </c>
       <c r="I322">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
@@ -10542,13 +10541,13 @@
         <v>15</v>
       </c>
       <c r="G323">
-        <v>0.73138297872340396</v>
+        <v>0.98138297872340396</v>
       </c>
       <c r="H323">
-        <v>0.14627659574468099</v>
+        <v>0.69095744680851101</v>
       </c>
       <c r="I323">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.3">
@@ -10571,13 +10570,13 @@
         <v>15</v>
       </c>
       <c r="G324">
-        <v>0.73138297872340396</v>
+        <v>0.98138297872340396</v>
       </c>
       <c r="H324">
-        <v>0.14627659574468099</v>
+        <v>0.69095744680851101</v>
       </c>
       <c r="I324">
-        <v>0.22220744680851001</v>
+        <v>0.47451241134751798</v>
       </c>
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.3">
@@ -10600,13 +10599,13 @@
         <v>15</v>
       </c>
       <c r="G325">
-        <v>0.73138297872340396</v>
+        <v>0.98138297872340396</v>
       </c>
       <c r="H325">
-        <v>0.14627659574468099</v>
+        <v>0.69095744680851101</v>
       </c>
       <c r="I325">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.3">
@@ -10629,13 +10628,13 @@
         <v>15</v>
       </c>
       <c r="G326">
-        <v>0.73138297872340396</v>
+        <v>0.98138297872340396</v>
       </c>
       <c r="H326">
-        <v>0.14627659574468099</v>
+        <v>0.69095744680851101</v>
       </c>
       <c r="I326">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.3">
@@ -10658,13 +10657,13 @@
         <v>15</v>
       </c>
       <c r="G327">
-        <v>0.73138297872340396</v>
+        <v>0.98138297872340396</v>
       </c>
       <c r="H327">
-        <v>0.14627659574468099</v>
+        <v>0.69095744680851101</v>
       </c>
       <c r="I327">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
@@ -10687,13 +10686,13 @@
         <v>15</v>
       </c>
       <c r="G328">
-        <v>0.73138297872340396</v>
+        <v>0.98138297872340396</v>
       </c>
       <c r="H328">
-        <v>0.14627659574468099</v>
+        <v>0.69095744680851101</v>
       </c>
       <c r="I328">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
@@ -10716,13 +10715,13 @@
         <v>15</v>
       </c>
       <c r="G329">
-        <v>0.73138297872340396</v>
+        <v>0.98138297872340396</v>
       </c>
       <c r="H329">
-        <v>0.14627659574468099</v>
+        <v>0.69095744680851101</v>
       </c>
       <c r="I329">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
@@ -10745,13 +10744,13 @@
         <v>15</v>
       </c>
       <c r="G330">
-        <v>0.73138297872340396</v>
+        <v>0.99468085106382897</v>
       </c>
       <c r="H330">
-        <v>7.4465974332995899E-2</v>
+        <v>0.58803191489361695</v>
       </c>
       <c r="I330">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
@@ -10774,13 +10773,13 @@
         <v>15</v>
       </c>
       <c r="G331">
-        <v>0.73138297872340396</v>
+        <v>0.99468085106382897</v>
       </c>
       <c r="H331">
-        <v>7.4465974332995899E-2</v>
+        <v>0.58803191489361695</v>
       </c>
       <c r="I331">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.3">
@@ -10803,13 +10802,13 @@
         <v>15</v>
       </c>
       <c r="G332">
-        <v>0.73138297872340396</v>
+        <v>0.99468085106382897</v>
       </c>
       <c r="H332">
-        <v>7.4465974332995899E-2</v>
+        <v>0.59015957446808498</v>
       </c>
       <c r="I332">
-        <v>0.22220744680851001</v>
+        <v>0.47451241134751798</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.3">
@@ -10832,13 +10831,13 @@
         <v>15</v>
       </c>
       <c r="G333">
-        <v>0.73138297872340396</v>
+        <v>0.99468085106382897</v>
       </c>
       <c r="H333">
-        <v>7.4465974332995899E-2</v>
+        <v>0.58803191489361695</v>
       </c>
       <c r="I333">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.3">
@@ -10861,13 +10860,13 @@
         <v>15</v>
       </c>
       <c r="G334">
-        <v>0.73138297872340396</v>
+        <v>0.99468085106382897</v>
       </c>
       <c r="H334">
-        <v>7.4465974332995899E-2</v>
+        <v>0.58803191489361695</v>
       </c>
       <c r="I334">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.3">
@@ -10890,13 +10889,13 @@
         <v>15</v>
       </c>
       <c r="G335">
-        <v>0.73138297872340396</v>
+        <v>0.99468085106382897</v>
       </c>
       <c r="H335">
-        <v>7.4465974332995899E-2</v>
+        <v>0.58803191489361695</v>
       </c>
       <c r="I335">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.3">
@@ -10919,13 +10918,13 @@
         <v>15</v>
       </c>
       <c r="G336">
-        <v>0.73138297872340396</v>
+        <v>0.99468085106382897</v>
       </c>
       <c r="H336">
-        <v>7.4465974332995899E-2</v>
+        <v>0.58803191489361695</v>
       </c>
       <c r="I336">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.3">
@@ -10948,13 +10947,13 @@
         <v>15</v>
       </c>
       <c r="G337">
-        <v>0.73138297872340396</v>
+        <v>0.99468085106382897</v>
       </c>
       <c r="H337">
-        <v>7.4465974332995899E-2</v>
+        <v>0.58803191489361695</v>
       </c>
       <c r="I337">
-        <v>0.22220744680851001</v>
+        <v>0.48958333333333298</v>
       </c>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.3">
@@ -21050,9 +21049,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F685" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F685"/>
   <hyperlinks>
-    <hyperlink ref="H1" r:id="rId1" display="P@k " xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H1" r:id="rId1" display="P@k "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>